<commit_message>
added 12V fuse. added ground planes to PCB and did nortons analysis on critical ground currents. https://github.com/neilh10/SensorModbusMaster/issues/1
</commit_message>
<xml_diff>
--- a/knh002-MayflyWingShield/rev4draft/KNH002rev4bomAA.xlsx
+++ b/knh002-MayflyWingShield/rev4draft/KNH002rev4bomAA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\usr\a\n\Netsensor\NetworkedSensors\projects\ccts\KNH002-rs485hyrbrid\K002rev4\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AF423E-1DB9-4341-9A02-57226A06EE65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7677D24E-4D3D-4399-81E3-1D2179EA9EB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="180" windowWidth="25665" windowHeight="19095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="180" windowWidth="25665" windowHeight="19095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="BuildNam">Header!$C$6</definedName>
     <definedName name="BuildQty">Header!$C$7</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Parts!$B$2:$L$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Parts!$B$2:$L$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="160">
   <si>
     <t>Source:</t>
   </si>
@@ -506,6 +506,21 @@
   </si>
   <si>
     <t>Basic build with external LiIon battery connections</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">507-1818-1-ND  </t>
+  </si>
+  <si>
+    <t>0ZCM0010FF2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUSE PTC 100MA </t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1435,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5710DB-CD36-4D48-83B7-3B63B6990DCD}">
-  <dimension ref="B1:P38"/>
+  <dimension ref="B1:P39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,66 +1875,60 @@
       <c r="C14" s="24"/>
       <c r="D14" s="37"/>
       <c r="E14" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>66</v>
+        <v>155</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>51</v>
+        <v>156</v>
+      </c>
+      <c r="H14" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" t="s">
+        <v>158</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="23"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="24"/>
       <c r="D15" s="37"/>
       <c r="E15" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="23"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>2</v>
@@ -1930,34 +1939,34 @@
       <c r="C16" s="24"/>
       <c r="D16" s="37"/>
       <c r="E16" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="23"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
@@ -1965,91 +1974,108 @@
       <c r="C17" s="24"/>
       <c r="D17" s="37"/>
       <c r="E17" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1</v>
+        <v>75</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>141</v>
+        <v>88</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="23"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="24"/>
       <c r="D18" s="37"/>
       <c r="E18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="3" t="str">
-        <f>I18</f>
-        <v>Wire 19AWG 10"</v>
+        <v>102</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="23"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="24"/>
       <c r="D19" s="37"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="E19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="3" t="str">
+        <f>I19</f>
+        <v>Wire 19AWG 10"</v>
+      </c>
       <c r="K19" s="3"/>
       <c r="L19" s="23"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="38"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="32" t="s">
-        <v>112</v>
-      </c>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -2062,16 +2088,11 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>55</v>
+      <c r="C21" s="43"/>
+      <c r="D21" s="38"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="32" t="s">
+        <v>112</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -2088,23 +2109,17 @@
       <c r="C22" s="24"/>
       <c r="D22" s="37"/>
       <c r="E22" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="23"/>
       <c r="M22" s="1"/>
@@ -2114,13 +2129,26 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="38"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="23"/>
       <c r="M23" s="1"/>
@@ -2130,13 +2158,10 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="19"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="15"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="38"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -2151,24 +2176,14 @@
       <c r="B25" s="19"/>
       <c r="C25" s="24"/>
       <c r="D25" s="37"/>
-      <c r="E25" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="23"/>
       <c r="M25" s="1"/>
@@ -2176,15 +2191,28 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="38"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="23"/>
       <c r="M26" s="1"/>
@@ -2192,15 +2220,12 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="19"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="15"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="38"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="33" t="s">
-        <v>113</v>
-      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -2215,24 +2240,14 @@
       <c r="B28" s="19"/>
       <c r="C28" s="24"/>
       <c r="D28" s="37"/>
-      <c r="E28" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>108</v>
-      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="23"/>
       <c r="M28" s="1"/>
@@ -2245,22 +2260,22 @@
       <c r="C29" s="24"/>
       <c r="D29" s="37"/>
       <c r="E29" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F29" s="4">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="23"/>
@@ -2269,15 +2284,28 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="19"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="38"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="L30" s="23"/>
       <c r="M30" s="1"/>
@@ -2285,15 +2313,12 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="15"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="38"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="33" t="s">
-        <v>114</v>
-      </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -2308,24 +2333,14 @@
       <c r="B32" s="19"/>
       <c r="C32" s="24"/>
       <c r="D32" s="37"/>
-      <c r="E32" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="4">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="23"/>
       <c r="M32" s="1"/>
@@ -2338,18 +2353,22 @@
       <c r="C33" s="24"/>
       <c r="D33" s="37"/>
       <c r="E33" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F33" s="4">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="J33" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="23"/>
@@ -2358,15 +2377,24 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="38"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="3"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="K34" s="3"/>
       <c r="L34" s="23"/>
       <c r="M34" s="1"/>
@@ -2374,15 +2402,12 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="15"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="38"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="33" t="s">
-        <v>132</v>
-      </c>
+      <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -2397,33 +2422,52 @@
       <c r="B36" s="19"/>
       <c r="C36" s="24"/>
       <c r="D36" s="37"/>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="15"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="19"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5" t="s">
+      <c r="F37" s="6"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K36" s="5"/>
-      <c r="L36" s="24"/>
-    </row>
-    <row r="37" spans="2:16" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="20"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="25"/>
-    </row>
-    <row r="38" spans="2:16" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="24"/>
+    </row>
+    <row r="38" spans="2:16" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="20"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="25"/>
+    </row>
+    <row r="39" spans="2:16" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2590,141 +2634,141 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>Parts!F14*BuildQty</f>
+        <f>Parts!F15*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B11" t="str">
-        <f>Parts!H14</f>
+        <f>Parts!H15</f>
         <v>175-MAX22025AWA+-ND</v>
       </c>
       <c r="C11" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E14," ",Parts!G14," ",Parts!J14)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E15," ",Parts!G15," ",Parts!J15)</f>
         <v>KNH2r4#9 U1 RS485 I/F</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>Parts!F15*BuildQty</f>
+        <f>Parts!F16*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B12" t="str">
-        <f>Parts!H15</f>
+        <f>Parts!H16</f>
         <v>2183-2117-ND</v>
       </c>
       <c r="C12" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E15," ",Parts!G15," ",Parts!J15)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E16," ",Parts!G16," ",Parts!J16)</f>
         <v>KNH2r4#10 U2 Bst 12V</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>Parts!F16*BuildQty</f>
+        <f>Parts!F17*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B13" t="str">
-        <f>Parts!H16</f>
+        <f>Parts!H17</f>
         <v>SIP32431DR3-T1GE3CT-ND</v>
       </c>
       <c r="C13" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E16," ",Parts!G16," ",Parts!J16)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E17," ",Parts!G17," ",Parts!J17)</f>
         <v>KNH2r4#11 U3 Switch</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>Parts!F17*BuildQty</f>
+        <f>Parts!F18*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B14" t="str">
-        <f>Parts!H17</f>
+        <f>Parts!H18</f>
         <v>296-SN74LVC2G34DCK3CT-ND</v>
       </c>
       <c r="C14" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E17," ",Parts!G17," ",Parts!J17)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E18," ",Parts!G18," ",Parts!J18)</f>
         <v>KNH2r4#12 U4 Buff Ioff</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>Parts!F18*BuildQty</f>
+        <f>Parts!F19*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B15" t="str">
-        <f>Parts!H18</f>
+        <f>Parts!H19</f>
         <v>Mm 8251T4 18AWG Green 50Ft</v>
       </c>
       <c r="C15" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E18," ",Parts!G18," ",Parts!J18)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E19," ",Parts!G19," ",Parts!J19)</f>
         <v>KNH2r4#13 J11 Wire 19AWG 10"</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>Parts!F22*BuildQty</f>
+        <f>Parts!F23*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B16" t="str">
-        <f>Parts!H22</f>
+        <f>Parts!H23</f>
         <v>311-0.0HRCT-ND</v>
       </c>
       <c r="C16" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E22," ",Parts!G22," ",Parts!J22)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E23," ",Parts!G23," ",Parts!J23)</f>
         <v>KNH2r4#15 R1 option Zero</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>Parts!F25*BuildQty</f>
+        <f>Parts!F26*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B17" t="str">
-        <f>Parts!H25</f>
+        <f>Parts!H26</f>
         <v>311-0.0HRCT-ND</v>
       </c>
       <c r="C17" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E25," ",Parts!G25," ",Parts!J25)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E26," ",Parts!G26," ",Parts!J26)</f>
         <v>KNH2r4#16 R5 option Zero</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>Parts!F28*BuildQty</f>
+        <f>Parts!F29*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B18" t="str">
-        <f>Parts!H28</f>
+        <f>Parts!H29</f>
         <v>273-KDV06FR100ETCT-ND</v>
       </c>
       <c r="C18" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E28," ",Parts!G28," ",Parts!J28)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E29," ",Parts!G29," ",Parts!J29)</f>
         <v>KNH2r4#17 R5 0.1ohm `%</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>Parts!F29*BuildQty</f>
+        <f>Parts!F30*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B19" t="str">
-        <f>Parts!H29</f>
+        <f>Parts!H30</f>
         <v>LTC2942IDCB-1#TRMPBFCT-ND</v>
       </c>
       <c r="C19" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E29," ",Parts!G29," ",Parts!J29)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E30," ",Parts!G30," ",Parts!J30)</f>
         <v>KNH2r4#18 U5 LTC2942</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>Parts!F32*BuildQty</f>
+        <f>Parts!F33*BuildQty</f>
         <v>6</v>
       </c>
       <c r="B20" t="str">
-        <f>Parts!H32</f>
+        <f>Parts!H33</f>
         <v>S9339-ND</v>
       </c>
       <c r="C20" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E32," ",Parts!G32," ",Parts!J32)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E33," ",Parts!G33," ",Parts!J33)</f>
         <v xml:space="preserve">KNH2r4#19 Shunt RS485 shunt 2mm </v>
       </c>
     </row>
@@ -3011,111 +3055,111 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="str">
-        <f>Parts!F14</f>
+        <f>Parts!F15</f>
         <v>1</v>
       </c>
       <c r="B13" t="str">
-        <f>Parts!G14</f>
+        <f>Parts!G15</f>
         <v>U1</v>
       </c>
       <c r="C13" t="str">
-        <f>Parts!H14</f>
+        <f>Parts!H15</f>
         <v>175-MAX22025AWA+-ND</v>
       </c>
       <c r="D13" t="str">
-        <f>Parts!I14</f>
+        <f>Parts!I15</f>
         <v>MAX22025AWA+</v>
       </c>
       <c r="E13" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E14," ",Parts!G14," ",Parts!J14)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E15," ",Parts!G15," ",Parts!J15)</f>
         <v>KNH2r4#9 U1 RS485 I/F</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="str">
-        <f>Parts!F15</f>
+        <f>Parts!F16</f>
         <v>1</v>
       </c>
       <c r="B14" t="str">
-        <f>Parts!G15</f>
+        <f>Parts!G16</f>
         <v>U2</v>
       </c>
       <c r="C14" t="str">
-        <f>Parts!H15</f>
+        <f>Parts!H16</f>
         <v>2183-2117-ND</v>
       </c>
       <c r="D14" t="str">
-        <f>Parts!I15</f>
+        <f>Parts!I16</f>
         <v xml:space="preserve">Pololu U3V12F12 </v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E15," ",Parts!G15," ",Parts!J15)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E16," ",Parts!G16," ",Parts!J16)</f>
         <v>KNH2r4#10 U2 Bst 12V</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="str">
-        <f>Parts!F16</f>
+        <f>Parts!F17</f>
         <v>1</v>
       </c>
       <c r="B15" t="str">
-        <f>Parts!G16</f>
+        <f>Parts!G17</f>
         <v>U3</v>
       </c>
       <c r="C15" t="str">
-        <f>Parts!H16</f>
+        <f>Parts!H17</f>
         <v>SIP32431DR3-T1GE3CT-ND</v>
       </c>
       <c r="D15" t="str">
-        <f>Parts!I16</f>
+        <f>Parts!I17</f>
         <v>SIP32431DR3-T1GE3</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E16," ",Parts!G16," ",Parts!J16)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E17," ",Parts!G17," ",Parts!J17)</f>
         <v>KNH2r4#11 U3 Switch</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
-        <f>Parts!F17</f>
+        <f>Parts!F18</f>
         <v>1</v>
       </c>
       <c r="B16" t="str">
-        <f>Parts!G17</f>
+        <f>Parts!G18</f>
         <v>U4</v>
       </c>
       <c r="C16" t="str">
-        <f>Parts!H17</f>
+        <f>Parts!H18</f>
         <v>296-SN74LVC2G34DCK3CT-ND</v>
       </c>
       <c r="D16" t="str">
-        <f>Parts!I17</f>
+        <f>Parts!I18</f>
         <v>SN74LVC2G34DCK3</v>
       </c>
       <c r="E16" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E17," ",Parts!G17," ",Parts!J17)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E18," ",Parts!G18," ",Parts!J18)</f>
         <v>KNH2r4#12 U4 Buff Ioff</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="str">
-        <f>Parts!F18</f>
+        <f>Parts!F19</f>
         <v>1</v>
       </c>
       <c r="B17" t="str">
-        <f>Parts!G18</f>
+        <f>Parts!G19</f>
         <v>J11</v>
       </c>
       <c r="C17" t="str">
-        <f>Parts!H18</f>
+        <f>Parts!H19</f>
         <v>Mm 8251T4 18AWG Green 50Ft</v>
       </c>
       <c r="D17" t="str">
-        <f>Parts!I18</f>
+        <f>Parts!I19</f>
         <v>Wire 19AWG 10"</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE(BuildNam,"#",Parts!E18," ",Parts!G18," ",Parts!J18)</f>
+        <f>CONCATENATE(BuildNam,"#",Parts!E19," ",Parts!G19," ",Parts!J19)</f>
         <v>KNH2r4#13 J11 Wire 19AWG 10"</v>
       </c>
     </row>

</xml_diff>